<commit_message>
Add results visualization notebook
</commit_message>
<xml_diff>
--- a/inputs_test.xlsx
+++ b/inputs_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\anais\a.duc-martin\ETE\ete-equilibre-offre-demande\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55970AB9-EDD0-460A-99F2-ADB30A1C76CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2813AB-53EB-4671-944E-F192BBC5BECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSETS" sheetId="2" r:id="rId1"/>
@@ -253,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -261,7 +261,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q940"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -528,10 +527,10 @@
       <c r="I1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" t="s">
         <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -567,7 +566,7 @@
         <v>10000</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H2" s="1">
         <v>10</v>
@@ -617,10 +616,10 @@
         <v>10000</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H3" s="1">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -685,7 +684,7 @@
         <v>0.5</v>
       </c>
       <c r="M4" s="1">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="N4" s="1">
         <v>200</v>
@@ -2790,7 +2789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T529"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>